<commit_message>
Se soluciona Ticket 9988:QA- Gestion de recursos -Licencias (RRHH) - Genera Reporte: formato fecha es tipo texto, cambiar a fecha
</commit_message>
<xml_diff>
--- a/src/Sofco.WebApi/wwwroot/excelTemplates/license-report.xlsx
+++ b/src/Sofco.WebApi/wwwroot/excelTemplates/license-report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\Gaps\src\Sofco.WebApi\wwwroot\excelTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GAPS\Fuentes\GAPS\src\Sofco.WebApi\wwwroot\excelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -109,12 +109,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,16 +406,16 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="30.875" customWidth="1"/>
     <col min="3" max="3" width="32.875" customWidth="1"/>
-    <col min="4" max="4" width="16.375" customWidth="1"/>
-    <col min="5" max="5" width="13.125" customWidth="1"/>
-    <col min="6" max="6" width="13.875" customWidth="1"/>
+    <col min="4" max="4" width="16.375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="13.125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13.875" style="5" customWidth="1"/>
     <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.875" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
@@ -424,13 +432,13 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -450,9 +458,9 @@
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>

</xml_diff>